<commit_message>
Incorporated most comments from Guy, Eoin and David
</commit_message>
<xml_diff>
--- a/data/data_statement_C2.xlsx
+++ b/data/data_statement_C2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anubhav/Google Drive/GitHub/C2_comp_qnty/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA69DCC-6516-204E-B611-35CF19DF4C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE71C97-9621-C34F-8A34-BC61D59CA5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{CC02A8C7-8F3A-3948-BA46-D50EADA6B3D7}"/>
+    <workbookView xWindow="540" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{CC02A8C7-8F3A-3948-BA46-D50EADA6B3D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>Broadstone Stream</t>
   </si>
@@ -66,10 +66,28 @@
     <t>Coauthors:</t>
   </si>
   <si>
-    <t>Anubhav Gupta, Owen Petchey, Eoin O'Gorman, Guy Woodward, David Figueroa</t>
-  </si>
-  <si>
     <t>Empirical dataset of foodwebs</t>
+  </si>
+  <si>
+    <t>Coilaco</t>
+  </si>
+  <si>
+    <t>Guampoe</t>
+  </si>
+  <si>
+    <t>Trancura</t>
+  </si>
+  <si>
+    <t>Anubhav Gupta, Owen Petchey, Eoin O'Gorman, Guy Woodward, David Figueroa, Iwan</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5281/zenodo.5575040</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5281/zenodo.6655759</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5281/zenodo.6655771</t>
   </si>
 </sst>
 </file>
@@ -458,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C160F91C-3568-9E41-9556-1EFF30084CF9}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C10" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,7 +494,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -491,12 +509,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -529,19 +550,22 @@
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -550,17 +574,73 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{DE1A5683-ADC0-A04B-9576-B6552DB3F221}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{2AEE51B4-F84E-5F40-96B2-D3C4DEA4BF69}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{BB94CE77-6253-A643-A42C-20BB6A9F8D11}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{DD4A2C26-CC05-064C-B0EE-4B432939F371}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{EED83C45-A7E2-1B4D-ACD6-AF517D5FD58B}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{641824F7-3AD1-F94E-BB0E-AD5B08293C3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>